<commit_message>
Rework Ovfl logic for CSA, fully completed and verified testbench for CSA.
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -258,10 +258,25 @@
     <t xml:space="preserve">DP1.0 Report Outine: Insert proper cover page, prepared report outline for resubmission.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Implemented and added conditional sum adder for Part 3) of DP1.</t>
+    <t xml:space="preserve">DP1.1: Implemented and added conditional sum adder topology (CSA) for Part 3a) of DP1.</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.1: Renamed CSA to CSAN, RippleAddr to RCAN, for consistent naming. Added initial Testbench files for the two topologies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Created Utils.vhd for utility functions. Added functions hex_to_slv, slv_to_hex, to enable easy translation between std_logic_vector typed values and hexadecimal values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Implemented features for Testbenches TBRCAN, TBCSAN: Added test vector processing via reading line by line from Adder00.tvs as well as logging to terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Added Ovfl output for CSA. Logic: check if the leftmost used adder overflowed or not: use that as the overflow of the whole CSA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1:  Fully completed DP1.1 3b): implemented stimulus application, verified correct results, implemented detailed failure logging, implemented writing into a transcript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Rework Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
   </si>
   <si>
     <r>
@@ -1364,7 +1379,7 @@
   <dimension ref="A1:I783"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1636,67 +1651,117 @@
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="31"/>
+      <c r="B14" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="29" t="n">
+        <v>46066</v>
+      </c>
+      <c r="D14" s="21" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E14" s="31" t="n">
+        <v>0.739583333333333</v>
+      </c>
       <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="G14" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="H14" s="34" t="n">
         <f aca="false">(E14-D14)*24</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="31"/>
+      <c r="B15" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="29" t="n">
+        <v>46066</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>0.739583333333333</v>
+      </c>
+      <c r="E15" s="31" t="n">
+        <v>0.791666666666667</v>
+      </c>
       <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="G15" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="H15" s="34" t="n">
         <f aca="false">(E15-D15)*24</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="31"/>
+      <c r="B16" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="29" t="n">
+        <v>46066</v>
+      </c>
+      <c r="D16" s="31" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E16" s="31" t="n">
+        <v>0.8125</v>
+      </c>
       <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="G16" s="33" t="s">
+        <v>25</v>
+      </c>
       <c r="H16" s="34" t="n">
         <f aca="false">(E16-D16)*24</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="31"/>
+      <c r="B17" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="29" t="n">
+        <v>46066</v>
+      </c>
+      <c r="D17" s="31" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="E17" s="31" t="n">
+        <v>0.895833333333333</v>
+      </c>
       <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="G17" s="33" t="s">
+        <v>26</v>
+      </c>
       <c r="H17" s="34" t="n">
         <f aca="false">(E17-D17)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="31"/>
+      <c r="B18" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D18" s="31" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E18" s="31" t="n">
+        <v>0.625</v>
+      </c>
       <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="G18" s="33" t="s">
+        <v>27</v>
+      </c>
       <c r="H18" s="34" t="n">
         <f aca="false">(E18-D18)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2496,7 +2561,7 @@
       <c r="F80" s="44"/>
       <c r="H80" s="45" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>13</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3271,7 +3336,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3292,7 +3357,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3305,7 +3370,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -5068,7 +5133,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5089,7 +5154,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -5102,7 +5167,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -6865,7 +6930,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -6886,7 +6951,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -6899,7 +6964,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -8662,7 +8727,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8683,7 +8748,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -8696,7 +8761,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -10441,7 +10506,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10459,7 +10524,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10480,7 +10545,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -10493,7 +10558,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>

</xml_diff>

<commit_message>
Corrected Part 2), fully completed testbenches.
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -258,25 +258,62 @@
     <t xml:space="preserve">DP1.0 Report Outine: Insert proper cover page, prepared report outline for resubmission.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Implemented and added conditional sum adder topology (CSA) for Part 3a) of DP1.</t>
+    <t xml:space="preserve">DP1.1: 3a) Implemented and added conditional sum adder topology (CSA) for Part 3a) of DP1.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Renamed CSA to CSAN, RippleAddr to RCAN, for consistent naming. Added initial Testbench files for the two topologies.</t>
+    <t xml:space="preserve">DP1.1: 3b) Renamed CSA to CSAN, RippleAddr to RCAN, for consistent naming. Added initial Testbench files for the two topologies.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Created Utils.vhd for utility functions. Added functions hex_to_slv, slv_to_hex, to enable easy translation between std_logic_vector typed values and hexadecimal values.</t>
+    <t xml:space="preserve">DP1.1: 3b) Created Utils.vhd for utility functions. Added functions hex_to_slv, slv_to_hex, to enable easy translation between std_logic_vector typed values and hexadecimal values.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Implemented features for Testbenches TBRCAN, TBCSAN: Added test vector processing via reading line by line from Adder00.tvs as well as logging to terminal.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DP1.1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3b): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Implemented features for Testbenches TBRCAN, TBCSAN: Added test vector processing via reading line by line from Adder00.tvs as well as logging to terminal.</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Added Ovfl output for CSA. Logic: check if the leftmost used adder overflowed or not: use that as the overflow of the whole CSA. Created 10  test vectors that fulfill functional verification testing requirements (Make sure that the inputs thoroughly test every part of the adder independently).</t>
+    <t xml:space="preserve">DP1.1: 3b) Added Ovfl output for CSA. Logic: check if the leftmost used adder overflowed or not: use that as the overflow of the whole CSA. Created 10  test vectors that fulfill functional verification testing requirements (Make sure that the inputs thoroughly test every part of the adder independently).</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1:  Fully completed DP1.1 3b): implemented stimulus application, verified correct results, implemented detailed failure logging, implemented writing into a transcript. Added 8 more test vectors, total of 18 test vectors used in the testbench.</t>
+    <t xml:space="preserve">DP1.1: 3b): implemented stimulus application, verified correct results, implemented detailed failure logging, implemented writing into a transcript. Added 8 more test vectors, total of 18 test vectors used in the testbench.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Rework Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
+    <t xml:space="preserve">DP1.1: 3a) Reworked Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 3b) Removed a line of code that was incorrectly trying to timestamp transcript file with the “now” keyword.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 2a) Fixed Baseline and FastRipple Implementations: Correct incorrect labeling of Baseline architecture as Fastripple, and vice versa. Added overflow detection for Fastripple, and Baseline architectures. Added Cout calculation for Fastripple. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 3b) Fully completed Testbenches and .do scripts for both RCAN and CSAN. Ensured expected operation for both topologies. Rename wave.do for TBCSAN to “waveCSAN.do”, and rename wave.do for TBRCAN to “waveRCAN.do”.</t>
   </si>
   <si>
     <r>
@@ -540,7 +577,7 @@
     <numFmt numFmtId="169" formatCode="0.00"/>
     <numFmt numFmtId="170" formatCode="h:mm:ss"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +697,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -868,7 +911,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1011,6 +1054,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1379,7 +1426,7 @@
   <dimension ref="A1:I783"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1566,10 +1613,10 @@
         <v>46054</v>
       </c>
       <c r="D10" s="21" t="n">
-        <v>0.583333333333333</v>
+        <v>0.625</v>
       </c>
       <c r="E10" s="31" t="n">
-        <v>0.708333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="33" t="s">
@@ -1577,7 +1624,7 @@
       </c>
       <c r="H10" s="34" t="n">
         <f aca="false">(E10-D10)*24</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1589,10 +1636,10 @@
         <v>46064</v>
       </c>
       <c r="D11" s="21" t="n">
-        <v>0.583333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E11" s="31" t="n">
-        <v>0.666666666666667</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33" t="s">
@@ -1600,7 +1647,7 @@
       </c>
       <c r="H11" s="34" t="n">
         <f aca="false">(E11-D11)*24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1766,41 +1813,71 @@
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="31"/>
+      <c r="B19" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D19" s="31" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="36" t="n">
+        <v>0.631944444444444</v>
+      </c>
       <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="G19" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="H19" s="34" t="n">
         <f aca="false">(E19-D19)*24</f>
-        <v>0</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="31"/>
+      <c r="B20" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D20" s="36" t="n">
+        <v>0.631944444444444</v>
+      </c>
+      <c r="E20" s="31" t="n">
+        <v>0.673611111111111</v>
+      </c>
       <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="G20" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="34" t="n">
         <f aca="false">(E20-D20)*24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="31"/>
+      <c r="B21" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D21" s="36" t="n">
+        <v>0.673611111111111</v>
+      </c>
+      <c r="E21" s="31" t="n">
+        <v>0.715277777777778</v>
+      </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="G21" s="33" t="s">
+        <v>30</v>
+      </c>
       <c r="H21" s="34" t="n">
         <f aca="false">(E21-D21)*24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2545,23 +2622,23 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>19.5</v>
+        <v>18.6666666666667</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3336,7 +3413,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3357,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3370,7 +3447,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -4342,21 +4419,21 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
         <v>0</v>
       </c>
@@ -5133,7 +5210,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5154,7 +5231,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -5167,7 +5244,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -6139,21 +6216,21 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
         <v>0</v>
       </c>
@@ -6930,7 +7007,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -6951,7 +7028,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -6964,7 +7041,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -7936,21 +8013,21 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
         <v>0</v>
       </c>
@@ -8727,7 +8804,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8748,7 +8825,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -8761,7 +8838,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -9733,21 +9810,21 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
         <v>0</v>
       </c>
@@ -10506,7 +10583,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10524,7 +10601,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10545,7 +10622,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -10558,7 +10635,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -11530,21 +11607,21 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="n">
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="n">
         <f aca="false">(E79-D79)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="44"/>
-      <c r="H80" s="45" t="n">
+      <c r="F80" s="45"/>
+      <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fully finish Part 4.
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="41">
   <si>
     <r>
       <rPr>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">DP1.1: 3b): implemented stimulus application, verified correct results, implemented detailed failure logging, implemented writing into a transcript. Added 8 more test vectors, total of 18 test vectors used in the testbench.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: 3a) Reworked Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
+    <t xml:space="preserve">DP1.1: 3a) (Completion) Reworked Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.1: 3b) Removed a line of code that was incorrectly trying to timestamp transcript file with the “now” keyword.</t>
@@ -313,7 +313,13 @@
     <t xml:space="preserve">DP1.1: 2a) Fixed Baseline and FastRipple Implementations: Correct incorrect labeling of Baseline architecture as Fastripple, and vice versa. Added overflow detection for Fastripple, and Baseline architectures. Added Cout calculation for Fastripple. </t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: 3b) Fully completed Testbenches and .do scripts for both RCAN and CSAN. Ensured expected operation for both topologies. Rename wave.do for TBCSAN to “waveCSAN.do”, and rename wave.do for TBRCAN to “waveRCAN.do”.</t>
+    <t xml:space="preserve">DP1.1: 3b) (Completion) Fully completed Testbenches and .do scripts for both RCAN and CSAN. Ensured expected operation for both topologies. Rename wave.do for TBCSAN to “waveCSAN.do”, and rename wave.do for TBRCAN to “waveRCAN.do”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 3a)  Revert base case adder of CSA to full adder. Was originally at 4-bit ripple adders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 4) (Completion) Implement RCANfv.do, CSANfv.do, functional verification .do scripts as outined in the requirements. Could not figure out how to pass command line arguments: therefore capture_set, the flag used to determine whether the output would be captured into a transcript file or not, is set at the top of these .do scripts for the time being.</t>
   </si>
   <si>
     <r>
@@ -1425,8 +1431,8 @@
   </sheetPr>
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1882,28 +1888,48 @@
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="31"/>
+      <c r="B22" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D22" s="21" t="n">
+        <v>0.715277777777778</v>
+      </c>
+      <c r="E22" s="31" t="n">
+        <v>0.722222222222222</v>
+      </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="G22" s="33" t="s">
+        <v>31</v>
+      </c>
       <c r="H22" s="34" t="n">
         <f aca="false">(E22-D22)*24</f>
-        <v>0</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="31"/>
+      <c r="B23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D23" s="31" t="n">
+        <v>0.722222222222222</v>
+      </c>
+      <c r="E23" s="31" t="n">
+        <v>0.805555555555556</v>
+      </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="G23" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="H23" s="34" t="n">
         <f aca="false">(E23-D23)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2638,7 +2664,7 @@
       <c r="F80" s="45"/>
       <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>18.6666666666667</v>
+        <v>20.8333333333333</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3413,7 +3439,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3434,7 +3460,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3447,7 +3473,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -5210,7 +5236,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5231,7 +5257,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -5244,7 +5270,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -7007,7 +7033,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7028,7 +7054,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -7041,7 +7067,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -8804,7 +8830,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8825,7 +8851,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -8838,7 +8864,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -10583,7 +10609,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10601,7 +10627,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10622,7 +10648,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -10635,7 +10661,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>

</xml_diff>

<commit_message>
Small improvement allowing for easier toggling on/off of output capture
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">DP1.1: 3b): implemented stimulus application, verified correct results, implemented detailed failure logging, implemented writing into a transcript. Added 8 more test vectors, total of 18 test vectors used in the testbench.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: 3a) (Completion) Reworked Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
+    <t xml:space="preserve">DP1.1: 3a) (Completion) Reworked Ovfl detection logic of CSA (check that the addition of two negatives makes a positive and vice versa instead of checking leftmost adder Ovfl), make report statements in testbench only give extensive details about failures to improve conciseness. Create wave.do file for ease of future simulations.</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.1: 3b) Removed a line of code that was incorrectly trying to timestamp transcript file with the “now” keyword.</t>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t xml:space="preserve">DP1.1: 4) (Completion) Implement RCANfv.do, CSANfv.do, functional verification .do scripts as outined in the requirements. Could not figure out how to pass command line arguments: therefore capture_set, the flag used to determine whether the output would be captured into a transcript file or not, is set at the top of these .do scripts for the time being.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: 4) Small improvement: allow easy toggling on/off of whether output is captured into transcript or not via set ::capture_set 1/0 in vsim terminal. Default capture_set is 1</t>
   </si>
   <si>
     <r>
@@ -1431,8 +1434,8 @@
   </sheetPr>
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1934,15 +1937,25 @@
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="31"/>
+      <c r="B24" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="29" t="n">
+        <v>46067</v>
+      </c>
+      <c r="D24" s="31" t="n">
+        <v>0.805555555555556</v>
+      </c>
+      <c r="E24" s="31" t="n">
+        <v>0.826388888888889</v>
+      </c>
       <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="G24" s="33" t="s">
+        <v>33</v>
+      </c>
       <c r="H24" s="34" t="n">
         <f aca="false">(E24-D24)*24</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2664,7 +2677,7 @@
       <c r="F80" s="45"/>
       <c r="H80" s="46" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>20.8333333333333</v>
+        <v>21.3333333333333</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3439,7 +3452,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3460,7 +3473,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3473,7 +3486,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -5236,7 +5249,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5257,7 +5270,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -5270,7 +5283,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -7033,7 +7046,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7054,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -7067,7 +7080,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -8830,7 +8843,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8851,7 +8864,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -8864,7 +8877,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -10609,7 +10622,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10627,7 +10640,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10648,7 +10661,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -10661,7 +10674,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>

</xml_diff>

<commit_message>
Make output of functional verification one-liners
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">DP1.1: Make several utility scripts and programs: nuke.sh for cleaning of project directory of all unecessary files, genTVDP1-1 for generating test vectors, verifyTVDP1-1 for verifying the generated test vectors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Add RTL view images of the two topologies, as well as technology viewer post fit images of each design candidate</t>
   </si>
   <si>
     <r>
@@ -3312,7 +3315,7 @@
   <dimension ref="A1:AG783"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3743,14 +3746,22 @@
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="32"/>
+      <c r="C21" s="30" t="n">
+        <v>46068</v>
+      </c>
+      <c r="D21" s="22" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E21" s="32" t="n">
+        <v>0.625</v>
+      </c>
       <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
+      <c r="G21" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="H21" s="35" t="n">
         <f aca="false">(E21-D21)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4511,7 +4522,7 @@
       <c r="F80" s="46"/>
       <c r="H80" s="47" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>16.3333333333333</v>
+        <v>18.3333333333333</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5286,7 +5297,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -5307,7 +5318,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -5320,7 +5331,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -7108,7 +7119,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -7129,7 +7140,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -7142,7 +7153,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -8930,7 +8941,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -8951,7 +8962,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -8964,7 +8975,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -10734,7 +10745,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -10752,7 +10763,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -10773,7 +10784,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -10786,7 +10797,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>

</xml_diff>

<commit_message>
Deliverable 9: Ultimate output summary created, located in OutputFiles
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <r>
       <rPr>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t xml:space="preserve">DP1.1: Add more in-depth comments to all VHDL files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Create VHDL listing for deliverable 5) of DP1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Create Ultimate Output Summary for all design candidates for deliverable 9) of DP1.1</t>
   </si>
   <si>
     <r>
@@ -1413,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:AG783"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1665,9 +1671,7 @@
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="28"/>
-      <c r="B12" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="22"/>
       <c r="E12" s="32"/>
@@ -1680,9 +1684,7 @@
     </row>
     <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
@@ -1695,9 +1697,7 @@
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="28"/>
-      <c r="B14" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B14" s="29"/>
       <c r="C14" s="30"/>
       <c r="D14" s="22"/>
       <c r="E14" s="32"/>
@@ -1710,9 +1710,7 @@
     </row>
     <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="28"/>
-      <c r="B15" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="29"/>
       <c r="C15" s="30"/>
       <c r="D15" s="22"/>
       <c r="E15" s="32"/>
@@ -1725,9 +1723,7 @@
     </row>
     <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="28"/>
-      <c r="B16" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B16" s="29"/>
       <c r="C16" s="30"/>
       <c r="D16" s="32"/>
       <c r="E16" s="32"/>
@@ -1740,9 +1736,7 @@
     </row>
     <row r="17" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
-      <c r="B17" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B17" s="29"/>
       <c r="C17" s="30"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
@@ -1755,9 +1749,7 @@
     </row>
     <row r="18" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="28"/>
-      <c r="B18" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B18" s="29"/>
       <c r="C18" s="30"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
@@ -1770,9 +1762,7 @@
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="28"/>
-      <c r="B19" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="29"/>
       <c r="C19" s="30"/>
       <c r="D19" s="32"/>
       <c r="E19" s="37"/>
@@ -1785,9 +1775,7 @@
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="28"/>
-      <c r="B20" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B20" s="29"/>
       <c r="C20" s="30"/>
       <c r="D20" s="37"/>
       <c r="E20" s="32"/>
@@ -1800,9 +1788,7 @@
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="28"/>
-      <c r="B21" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B21" s="29"/>
       <c r="C21" s="30"/>
       <c r="D21" s="37"/>
       <c r="E21" s="32"/>
@@ -1815,9 +1801,7 @@
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="28"/>
-      <c r="B22" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B22" s="29"/>
       <c r="C22" s="30"/>
       <c r="D22" s="22"/>
       <c r="E22" s="32"/>
@@ -1830,9 +1814,7 @@
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="28"/>
-      <c r="B23" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B23" s="29"/>
       <c r="C23" s="30"/>
       <c r="D23" s="32"/>
       <c r="E23" s="32"/>
@@ -1845,9 +1827,7 @@
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="28"/>
-      <c r="B24" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B24" s="29"/>
       <c r="C24" s="30"/>
       <c r="D24" s="32"/>
       <c r="E24" s="32"/>
@@ -1860,9 +1840,7 @@
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="28"/>
-      <c r="B25" s="29" t="s">
-        <v>15</v>
-      </c>
+      <c r="B25" s="29"/>
       <c r="C25" s="30"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
@@ -3318,7 +3296,7 @@
   <dimension ref="A1:AG783"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3453,7 +3431,9 @@
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="C7" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3475,7 +3455,9 @@
     </row>
     <row r="8" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="B8" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3496,7 +3478,9 @@
     </row>
     <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
+      <c r="B9" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3517,7 +3501,9 @@
     </row>
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3538,7 +3524,9 @@
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
+      <c r="B11" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3559,7 +3547,9 @@
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
+      <c r="B12" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="30" t="n">
         <v>46066</v>
       </c>
@@ -3580,7 +3570,9 @@
     </row>
     <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
+      <c r="B13" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3601,7 +3593,9 @@
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
+      <c r="B14" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C14" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3622,7 +3616,9 @@
     </row>
     <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C15" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3643,7 +3639,9 @@
     </row>
     <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
+      <c r="B16" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3664,7 +3662,9 @@
     </row>
     <row r="17" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
+      <c r="B17" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="C17" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3685,7 +3685,9 @@
     </row>
     <row r="18" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3706,7 +3708,9 @@
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C19" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3727,7 +3731,9 @@
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
+      <c r="B20" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C20" s="30" t="n">
         <v>46067</v>
       </c>
@@ -3748,7 +3754,9 @@
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
+      <c r="B21" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="C21" s="30" t="n">
         <v>46068</v>
       </c>
@@ -3769,7 +3777,9 @@
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="C22" s="30" t="n">
         <v>46068</v>
       </c>
@@ -3790,28 +3800,48 @@
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="32"/>
+      <c r="B23" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="30" t="n">
+        <v>46068</v>
+      </c>
+      <c r="D23" s="22" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E23" s="32" t="n">
+        <v>0.791666666666667</v>
+      </c>
       <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
+      <c r="G23" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="H23" s="35" t="n">
         <f aca="false">(E23-D23)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="32"/>
+      <c r="B24" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="30" t="n">
+        <v>46068</v>
+      </c>
+      <c r="D24" s="32" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E24" s="32" t="n">
+        <v>0.875</v>
+      </c>
       <c r="F24" s="33"/>
-      <c r="G24" s="34"/>
+      <c r="G24" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="H24" s="35" t="n">
         <f aca="false">(E24-D24)*24</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4533,7 +4563,7 @@
       <c r="F80" s="46"/>
       <c r="H80" s="47" t="n">
         <f aca="false">SUM(H7:H79)</f>
-        <v>20.3333333333333</v>
+        <v>24.3333333333333</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5308,7 +5338,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -5329,7 +5359,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -5342,7 +5372,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -7130,7 +7160,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -7151,7 +7181,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -7164,7 +7194,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -8952,7 +8982,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -8973,7 +9003,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -8986,7 +9016,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -10756,7 +10786,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -10774,7 +10804,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -10795,7 +10825,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -10808,7 +10838,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>

</xml_diff>

<commit_message>
Deliverable 11: Document Name Summary Table
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G12-4645-350-1261.xlsx
+++ b/Documentation/ProjectLog-G12-4645-350-1261.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
   <si>
     <r>
       <rPr>
@@ -343,16 +343,19 @@
     <t xml:space="preserve">DP1.1: Make several utility scripts and programs: nuke.sh for cleaning of project directory of all unecessary files, genTVDP1-1 for generating test vectors, verifyTVDP1-1 for verifying the generated test vectors.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Add RTL view images of the two topologies, as well as technology viewer post fit images of each design candidate</t>
+    <t xml:space="preserve">DP1.1: Add RTL view images of the two topologies, as well as technology viewer post fit images of each design candidate. Rework output of testbench files to be one-liners, and create “append” utility function for concatenating strings together for better outputs.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Add more in-depth comments to all VHDL files</t>
+    <t xml:space="preserve">DP1.1: Add more in-depth comments to all VHDL files.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Create VHDL listing for deliverable 5) of DP1.1</t>
+    <t xml:space="preserve">DP1.1: Create VHDL listing for deliverable 5) of DP1.1.</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.1: Create Ultimate Output Summary for all design candidates for deliverable 9) of DP1.1</t>
+    <t xml:space="preserve">DP1.1: Complete Ultimate Output Summary (DP1-Quartus-Summary-G12-350-1261.txt) for all design candidates for deliverable 9) of DP1.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.1: Create Document Name Summary Table for deliverable 11) of DP1.1.</t>
   </si>
   <si>
     <r>
@@ -3295,8 +3298,8 @@
   </sheetPr>
   <dimension ref="A1:AG783"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C8" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3833,7 +3836,7 @@
         <v>0.791666666666667</v>
       </c>
       <c r="E24" s="32" t="n">
-        <v>0.875</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="34" t="s">
@@ -3841,20 +3844,30 @@
       </c>
       <c r="H24" s="35" t="n">
         <f aca="false">(E24-D24)*24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="30" t="n">
+        <v>46068</v>
+      </c>
+      <c r="D25" s="32" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E25" s="32" t="n">
+        <v>0.875</v>
+      </c>
       <c r="F25" s="33"/>
-      <c r="G25" s="34"/>
+      <c r="G25" s="34" t="s">
+        <v>40</v>
+      </c>
       <c r="H25" s="35" t="n">
         <f aca="false">(E25-D25)*24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5338,7 +5351,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -5359,7 +5372,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -5372,7 +5385,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -7160,7 +7173,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -7181,7 +7194,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -7194,7 +7207,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -8982,7 +8995,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -9003,7 +9016,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -9016,7 +9029,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -10786,7 +10799,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -10804,7 +10817,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -10825,7 +10838,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -10838,7 +10851,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>

</xml_diff>